<commit_message>
Updated hafele mdf door order loading tests
</commit_message>
<xml_diff>
--- a/Orders/OrderLoading/OrderLoading.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
+++ b/Orders/OrderLoading/OrderLoading.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Londono\source\repos\OrderProcessor\ApplicationCore\ApplicationCore.Tests.Unit\HafeleMDFDoorOrderLoading\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Londono\source\repos\OrderProcessor\Orders\OrderLoading\OrderLoading.Tests.Unit\HafeleMDFDoorOrderLoading\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE49F101-98DF-4AA2-8169-755BECC13C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A606601-ED75-40A4-9DC7-4CE5D5A0095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="1185" windowWidth="15255" windowHeight="13650" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
+    <workbookView xWindow="9030" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="3" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="177">
   <si>
     <t>Qty</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>Tracking Number</t>
+  </si>
+  <si>
+    <t>This is a comment</t>
   </si>
 </sst>
 </file>
@@ -1288,6 +1291,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1300,13 +1324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1346,21 +1364,6 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1549,7 +1552,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1889"/>
+                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1893"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1637,7 +1640,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1890"/>
+                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1894"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1725,7 +1728,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1891"/>
+                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1895"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3833,7 +3836,7 @@
   <dimension ref="B1:H45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B13" sqref="B13:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,10 +3859,10 @@
   <sheetData>
     <row r="1" spans="2:8" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="55"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
@@ -3886,13 +3889,13 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="71" t="str" cm="1">
+      <c r="B6" s="53" t="str" cm="1">
         <f t="array" ref="B6">"MDF Door Configurator      " &amp; WBVersion</f>
         <v>MDF Door Configurator      Beta 1.3</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
       <c r="G6" s="12" t="s">
         <v>39</v>
       </c>
@@ -3902,10 +3905,10 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="70"/>
+      <c r="D8" s="50"/>
       <c r="G8" s="5" t="s">
         <v>41</v>
       </c>
@@ -3939,22 +3942,24 @@
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="G12" s="53" t="s">
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="52"/>
+      <c r="G12" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="55"/>
+      <c r="H12" s="52"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
+      <c r="B13" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
       <c r="G13" s="5" t="s">
         <v>139</v>
       </c>
@@ -3963,10 +3968,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="59"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
       <c r="G14" s="24" t="s">
         <v>136</v>
       </c>
@@ -3975,10 +3980,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
       <c r="G15" s="6" t="s">
         <v>140</v>
       </c>
@@ -3988,10 +3993,10 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
       <c r="G16" s="6" t="s">
         <v>141</v>
       </c>
@@ -4001,10 +4006,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
       <c r="G17" s="24" t="s">
         <v>137</v>
       </c>
@@ -4013,10 +4018,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
       <c r="G18" s="6" t="s">
         <v>138</v>
       </c>
@@ -4025,10 +4030,10 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
       <c r="G19" s="6" t="s">
         <v>132</v>
       </c>
@@ -4072,12 +4077,12 @@
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="52"/>
       <c r="G25" s="42"/>
       <c r="H25" s="43"/>
     </row>
@@ -4085,11 +4090,11 @@
       <c r="B26" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="73"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="55"/>
       <c r="G26" s="8"/>
       <c r="H26" s="9"/>
     </row>
@@ -4097,11 +4102,11 @@
       <c r="B27" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="65" t="s">
+      <c r="C27" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="66"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="71"/>
       <c r="G27" s="8"/>
       <c r="H27" s="9"/>
     </row>
@@ -4109,11 +4114,11 @@
       <c r="B28" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="C28" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
       <c r="G28" s="8"/>
       <c r="H28" s="9"/>
     </row>
@@ -4121,11 +4126,11 @@
       <c r="B29" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="C29" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
       <c r="G29" s="8"/>
       <c r="H29" s="9"/>
     </row>
@@ -4133,11 +4138,11 @@
       <c r="B30" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="C30" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="65"/>
-      <c r="E30" s="66"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
       <c r="G30" s="8"/>
       <c r="H30" s="9"/>
     </row>
@@ -4145,11 +4150,11 @@
       <c r="B31" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="66"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="71"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
     </row>
@@ -4157,11 +4162,11 @@
       <c r="B32" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="65" t="s">
+      <c r="C32" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="66"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="71"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9"/>
     </row>
@@ -4169,11 +4174,11 @@
       <c r="B33" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="57"/>
       <c r="G33" s="8"/>
       <c r="H33" s="9"/>
     </row>
@@ -4181,11 +4186,11 @@
       <c r="B34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="67"/>
-      <c r="E34" s="68"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="73"/>
       <c r="G34" s="8"/>
       <c r="H34" s="9"/>
     </row>
@@ -4193,11 +4198,11 @@
       <c r="B35" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="57"/>
       <c r="G35" s="8"/>
       <c r="H35" s="9"/>
     </row>
@@ -4205,11 +4210,11 @@
       <c r="B36" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="49"/>
-      <c r="E36" s="50"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="57"/>
       <c r="G36" s="8"/>
       <c r="H36" s="9"/>
     </row>
@@ -4217,11 +4222,11 @@
       <c r="B37" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C37" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="51"/>
-      <c r="E37" s="52"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="59"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
     </row>
@@ -4259,11 +4264,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C26:E26"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B25:E25"/>
@@ -4278,6 +4278,11 @@
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <conditionalFormatting sqref="G20:H20">
     <cfRule type="expression" dxfId="11" priority="1">

</xml_diff>

<commit_message>
Read hafele markup and discount from data tab
</commit_message>
<xml_diff>
--- a/Orders/OrderLoading/OrderLoading.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
+++ b/Orders/OrderLoading/OrderLoading.Tests.Unit/HafeleMDFDoorOrderLoading/TestData/Test1.3.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary Londono\source\repos\OrderProcessor\Orders\OrderLoading\OrderLoading.Tests.Unit\HafeleMDFDoorOrderLoading\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A606601-ED75-40A4-9DC7-4CE5D5A0095B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A0AFC8-9EEE-4446-8AF2-2FEDB062C4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="1orCApCeaXQlP5C/jGRQRaerBK2Egt1ZWZbj43z6b9zKl6k2xLQSzylFzGYeoTmrbX6pQr/vGgb8BHRd6aPFHw==" workbookSaltValue="iFrGvnN01ynv4+4GF0kd9w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{055880C2-27AA-406A-A981-7BEBAEB91D4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Options" sheetId="3" r:id="rId1"/>
     <sheet name="Sizes" sheetId="1" r:id="rId2"/>
     <sheet name="Pictures" sheetId="5" r:id="rId3"/>
-    <sheet name="Data" sheetId="2" r:id="rId4"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Account_Number">Options!$C$28</definedName>
@@ -1291,27 +1292,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1324,7 +1304,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1364,6 +1350,21 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1552,7 +1553,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1893"/>
+                  <a14:cameraTool cellRange="Framing_Bead_Image" spid="_x0000_s1896"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1640,7 +1641,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1894"/>
+                  <a14:cameraTool cellRange="Edge_Profile_Image" spid="_x0000_s1897"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1728,7 +1729,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1895"/>
+                  <a14:cameraTool cellRange="Panel_Detail_Image" spid="_x0000_s1898"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3859,10 +3860,10 @@
   <sheetData>
     <row r="1" spans="2:8" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="52"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
@@ -3889,13 +3890,13 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53" t="str" cm="1">
+      <c r="B6" s="71" t="str" cm="1">
         <f t="array" ref="B6">"MDF Door Configurator      " &amp; WBVersion</f>
         <v>MDF Door Configurator      Beta 1.3</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
       <c r="G6" s="12" t="s">
         <v>39</v>
       </c>
@@ -3905,10 +3906,10 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="50"/>
+      <c r="D8" s="70"/>
       <c r="G8" s="5" t="s">
         <v>41</v>
       </c>
@@ -3942,24 +3943,24 @@
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="52"/>
-      <c r="G12" s="51" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+      <c r="G12" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="63"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
       <c r="G13" s="5" t="s">
         <v>139</v>
       </c>
@@ -3968,10 +3969,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="61"/>
       <c r="G14" s="24" t="s">
         <v>136</v>
       </c>
@@ -3980,10 +3981,10 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
       <c r="G15" s="6" t="s">
         <v>140</v>
       </c>
@@ -3993,10 +3994,10 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="64"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="G16" s="6" t="s">
         <v>141</v>
       </c>
@@ -4006,10 +4007,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="64"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="G17" s="24" t="s">
         <v>137</v>
       </c>
@@ -4018,10 +4019,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="64"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
       <c r="G18" s="6" t="s">
         <v>138</v>
       </c>
@@ -4030,10 +4031,10 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="69"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
       <c r="G19" s="6" t="s">
         <v>132</v>
       </c>
@@ -4077,12 +4078,12 @@
     <row r="23" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="52"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="55"/>
       <c r="G25" s="42"/>
       <c r="H25" s="43"/>
     </row>
@@ -4090,11 +4091,11 @@
       <c r="B26" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="54"/>
-      <c r="E26" s="55"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="73"/>
       <c r="G26" s="8"/>
       <c r="H26" s="9"/>
     </row>
@@ -4102,11 +4103,11 @@
       <c r="B27" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="71"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="66"/>
       <c r="G27" s="8"/>
       <c r="H27" s="9"/>
     </row>
@@ -4114,11 +4115,11 @@
       <c r="B28" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
       <c r="G28" s="8"/>
       <c r="H28" s="9"/>
     </row>
@@ -4126,11 +4127,11 @@
       <c r="B29" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="70" t="s">
+      <c r="C29" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="71"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
       <c r="G29" s="8"/>
       <c r="H29" s="9"/>
     </row>
@@ -4138,11 +4139,11 @@
       <c r="B30" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="70" t="s">
+      <c r="C30" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="66"/>
       <c r="G30" s="8"/>
       <c r="H30" s="9"/>
     </row>
@@ -4150,11 +4151,11 @@
       <c r="B31" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C31" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="71"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
       <c r="G31" s="10"/>
       <c r="H31" s="11"/>
     </row>
@@ -4162,11 +4163,11 @@
       <c r="B32" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="70" t="s">
+      <c r="C32" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="71"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="66"/>
       <c r="G32" s="8"/>
       <c r="H32" s="9"/>
     </row>
@@ -4174,11 +4175,11 @@
       <c r="B33" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
       <c r="G33" s="8"/>
       <c r="H33" s="9"/>
     </row>
@@ -4186,11 +4187,11 @@
       <c r="B34" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="72"/>
-      <c r="E34" s="73"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="68"/>
       <c r="G34" s="8"/>
       <c r="H34" s="9"/>
     </row>
@@ -4198,11 +4199,11 @@
       <c r="B35" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="56"/>
-      <c r="E35" s="57"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
       <c r="G35" s="8"/>
       <c r="H35" s="9"/>
     </row>
@@ -4210,11 +4211,11 @@
       <c r="B36" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
       <c r="G36" s="8"/>
       <c r="H36" s="9"/>
     </row>
@@ -4222,11 +4223,11 @@
       <c r="B37" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52"/>
       <c r="G37" s="8"/>
       <c r="H37" s="9"/>
     </row>
@@ -4264,6 +4265,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="B25:E25"/>
@@ -4278,18 +4284,13 @@
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <conditionalFormatting sqref="G20:H20">
     <cfRule type="expression" dxfId="11" priority="1">
       <formula>NOT(_xlfn.XLOOKUP(Finish_Type, Finish_Types, Finish_Types_Has_Color, FALSE, 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="9">
+  <dataValidations disablePrompts="1" count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L8" xr:uid="{B2265125-E5E1-44F6-A2F5-0FE434E6F6AB}">
       <formula1>Framing_Beads</formula1>
     </dataValidation>
@@ -11905,7 +11906,7 @@
   <dimension ref="B2:AO33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>